<commit_message>
modify of sheet excel
</commit_message>
<xml_diff>
--- a/Patrones de Comportamiento/Interpreter/src/META_INF/Employee.xlsx
+++ b/Patrones de Comportamiento/Interpreter/src/META_INF/Employee.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="hoja 1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -52,9 +52,6 @@
     <t xml:space="preserve">Sistemas</t>
   </si>
   <si>
-    <t xml:space="preserve">10/20/1981</t>
-  </si>
-  <si>
     <t xml:space="preserve">Activo</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
     <t xml:space="preserve">Contabilidad</t>
   </si>
   <si>
-    <t xml:space="preserve">10/20/1990</t>
-  </si>
-  <si>
     <t xml:space="preserve">Baja</t>
   </si>
   <si>
@@ -82,9 +76,6 @@
     <t xml:space="preserve">Finanzas</t>
   </si>
   <si>
-    <t xml:space="preserve">10/20/1976</t>
-  </si>
-  <si>
     <t xml:space="preserve">Juan</t>
   </si>
   <si>
@@ -94,9 +85,6 @@
     <t xml:space="preserve">Compras</t>
   </si>
   <si>
-    <t xml:space="preserve">10/20/1989</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bairon</t>
   </si>
   <si>
@@ -110,9 +98,6 @@
   </si>
   <si>
     <t xml:space="preserve">Castillo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09/21/1989</t>
   </si>
 </sst>
 </file>
@@ -146,12 +131,24 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFD095"/>
+        <bgColor rgb="FF99CCFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -188,7 +185,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -197,12 +194,28 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -214,6 +227,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFAFD095"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -225,7 +298,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -240,163 +313,163 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="6" t="n">
+        <v>36492</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="5" t="n">
+        <v>8374953759</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="0" t="n">
-        <v>8374953759</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="6" t="n">
+        <v>36493</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="G3" s="5" t="n">
+        <v>8429349242</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="C4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="0" t="n">
-        <v>8429349242</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="s">
+      <c r="D4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="E4" s="6" t="n">
+        <v>36494</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>29840298</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="C5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="D5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>29840298</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="0" t="s">
+      <c r="E5" s="6" t="n">
+        <v>36495</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>9982934820</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E6" s="6" t="n">
+        <v>36496</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>990121525</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>9982934820</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="0" t="s">
+      <c r="C7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="3" t="n">
-        <v>36496</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>990121525</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="0" t="n">
+      <c r="D7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="6" t="n">
+        <v>36497</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="5" t="n">
         <v>9812413536</v>
       </c>
     </row>

</xml_diff>